<commit_message>
se agregaron las ultimas mejoras a las tres paginas
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eaddfdadc636372/Escritorio/experiencia1_tobar_002D/experiencia1_tobar_002D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42B26A20-501D-4088-BF52-6751E201EB95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{42B26A20-501D-4088-BF52-6751E201EB95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{16BC9DDB-225C-424B-B858-21AEEA6BCB6D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{FCDE2450-F88F-495E-B1FA-0A36D45218BF}"/>
   </bookViews>
   <sheets>
     <sheet name="BitácoraExperiencia1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Equipo</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">realice el ultimo commit </t>
-  </si>
-  <si>
-    <t>envie el proyecto a la profesora</t>
   </si>
 </sst>
 </file>
@@ -459,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA7284-98DD-4C9B-85C9-6827807F75AB}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -625,17 +622,6 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>